<commit_message>
Interfaz de Encuesta, boton submit anulado
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-encuesta.xlsx
+++ b/assets/info/plantilla-encuesta.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="RESPUESTAS" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ENCUESTAS" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RESPUESTAS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t xml:space="preserve">REPORTES ENCUESTAS</t>
   </si>
@@ -49,19 +50,34 @@
     <t xml:space="preserve">CODIGO</t>
   </si>
   <si>
+    <t xml:space="preserve">USUARIO</t>
+  </si>
+  <si>
     <t xml:space="preserve">LATITUD</t>
   </si>
   <si>
     <t xml:space="preserve">LONGITUD</t>
   </si>
   <si>
+    <t xml:space="preserve">EDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEXO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AREA</t>
+  </si>
+  <si>
     <t xml:space="preserve">CIUDAD</t>
   </si>
   <si>
     <t xml:space="preserve">ZONA</t>
   </si>
   <si>
-    <t xml:space="preserve">USUARIO</t>
+    <t xml:space="preserve">TIEMPO[min]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIEMPO</t>
   </si>
   <si>
     <t xml:space="preserve">MODULO</t>
@@ -209,7 +225,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,7 +239,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -242,10 +266,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,10 +287,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,6 +300,14 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -393,9 +417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>730080</xdr:colOff>
+      <xdr:colOff>728280</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>226440</xdr:rowOff>
+      <xdr:rowOff>224640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -409,7 +433,49 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="309960"/>
-          <a:ext cx="3333600" cy="1301400"/>
+          <a:ext cx="3331800" cy="1299600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>728280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>225360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Imagen 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66600" y="310680"/>
+          <a:ext cx="3331800" cy="1299600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -431,8 +497,8 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,91 +511,110 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="44.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="61.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="41.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="61.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="58.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="48.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="43.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="5" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="48.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="37.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="7" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D3" s="9" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="7"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" s="5" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="13" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" s="5" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" s="5" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="14"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
@@ -598,4 +683,190 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="44.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="39.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="19" width="44.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="19" width="52.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="19" width="61.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="41.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="58.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="7" width="48.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="37.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="7" width="44.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="7" width="11.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="20"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" s="7" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" s="7" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="14"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G11:G1048576 G1">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G1048576 G1:G9">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("Censo",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Administrador de encuesta implementado, reporte pendiente
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-encuesta.xlsx
+++ b/assets/info/plantilla-encuesta.xlsx
@@ -417,9 +417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>224640</xdr:rowOff>
+      <xdr:rowOff>224280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -433,7 +433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="309960"/>
-          <a:ext cx="3331800" cy="1299600"/>
+          <a:ext cx="3331440" cy="1299240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -459,9 +459,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>225360</xdr:rowOff>
+      <xdr:rowOff>225000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,7 +475,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="310680"/>
-          <a:ext cx="3331800" cy="1299600"/>
+          <a:ext cx="3331440" cy="1299240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>